<commit_message>
Ispravke, kolega Anja da pregleda sve
</commit_message>
<xml_diff>
--- a/2b Format partner budget - Horizon2020  VIZLORE .xlsx
+++ b/2b Format partner budget - Horizon2020  VIZLORE .xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Anja\Fakultet\6. semestar\USP\Projekat\Projekat\Projekat_Faza1_ver1\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9189"/>
   </bookViews>
   <sheets>
     <sheet name="Detaljno budzet" sheetId="1" r:id="rId1"/>
@@ -20,7 +15,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Travel - budzet'!$B$4:$P$46</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="98">
   <si>
     <t>Partner budget Horizon 2020</t>
   </si>
@@ -323,12 +318,18 @@
   </si>
   <si>
     <t>isto kao pored ako je reasearch</t>
+  </si>
+  <si>
+    <t>WP1</t>
+  </si>
+  <si>
+    <t>Athens</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
@@ -696,7 +697,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -816,6 +817,11 @@
     <xf numFmtId="0" fontId="13" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -896,10 +902,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -946,7 +948,7 @@
         <xdr:cNvPr id="3" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA4F558B-8D56-430D-AA83-772AD1DE26DE}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA4F558B-8D56-430D-AA83-772AD1DE26DE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1048,7 +1050,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1083,7 +1085,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1298,10 +1300,10 @@
   <dimension ref="A1:T39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.65" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.44140625" customWidth="1"/>
     <col min="2" max="2" width="24.77734375" customWidth="1"/>
@@ -1316,77 +1318,77 @@
     <col min="15" max="19" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="24.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="25.05" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="83"/>
+      <c r="I3" s="83"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D4" s="2"/>
-      <c r="E4" s="81" t="s">
+      <c r="E4" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="82"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="85"/>
       <c r="J4" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="L4" s="82" t="s">
+      <c r="L4" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="82"/>
-      <c r="N4" s="82"/>
+      <c r="M4" s="85"/>
+      <c r="N4" s="85"/>
       <c r="O4" s="4">
         <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D5" s="2"/>
-      <c r="E5" s="81" t="s">
+      <c r="E5" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="82"/>
-      <c r="G5" s="82"/>
-      <c r="H5" s="82"/>
-      <c r="I5" s="82"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="85"/>
+      <c r="H5" s="85"/>
+      <c r="I5" s="85"/>
       <c r="J5" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="L5" s="82" t="s">
+      <c r="L5" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="M5" s="82"/>
-      <c r="N5" s="82"/>
+      <c r="M5" s="85"/>
+      <c r="N5" s="85"/>
       <c r="O5" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D6" s="2"/>
-      <c r="E6" s="81" t="s">
+      <c r="E6" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="82"/>
-      <c r="G6" s="82"/>
-      <c r="H6" s="82"/>
-      <c r="I6" s="82"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="85"/>
       <c r="J6" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="L6" s="82" t="s">
+      <c r="L6" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="M6" s="82"/>
-      <c r="N6" s="82"/>
+      <c r="M6" s="85"/>
+      <c r="N6" s="85"/>
       <c r="O6" s="5">
         <v>0.7</v>
       </c>
@@ -1396,21 +1398,21 @@
       <c r="Q6" s="6"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="E7" s="82" t="s">
+      <c r="E7" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="82"/>
+      <c r="F7" s="85"/>
+      <c r="G7" s="85"/>
+      <c r="H7" s="85"/>
+      <c r="I7" s="85"/>
       <c r="J7" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="L7" s="82" t="s">
+      <c r="L7" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="82"/>
-      <c r="N7" s="82"/>
+      <c r="M7" s="85"/>
+      <c r="N7" s="85"/>
       <c r="O7" s="4">
         <v>1</v>
       </c>
@@ -1419,58 +1421,58 @@
       <c r="J8" s="2"/>
       <c r="O8" s="7"/>
     </row>
-    <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="83" t="s">
+    <row r="9" spans="1:19" ht="15.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="84"/>
-      <c r="C10" s="84"/>
-      <c r="D10" s="84"/>
-      <c r="E10" s="84"/>
-      <c r="F10" s="84"/>
-      <c r="G10" s="84"/>
-      <c r="H10" s="84"/>
-      <c r="I10" s="84"/>
-      <c r="J10" s="84"/>
-      <c r="K10" s="84"/>
-      <c r="L10" s="84"/>
-      <c r="M10" s="84"/>
-      <c r="N10" s="84"/>
-      <c r="O10" s="84"/>
-      <c r="P10" s="84"/>
-      <c r="Q10" s="84"/>
-      <c r="R10" s="84"/>
+      <c r="B10" s="87"/>
+      <c r="C10" s="87"/>
+      <c r="D10" s="87"/>
+      <c r="E10" s="87"/>
+      <c r="F10" s="87"/>
+      <c r="G10" s="87"/>
+      <c r="H10" s="87"/>
+      <c r="I10" s="87"/>
+      <c r="J10" s="87"/>
+      <c r="K10" s="87"/>
+      <c r="L10" s="87"/>
+      <c r="M10" s="87"/>
+      <c r="N10" s="87"/>
+      <c r="O10" s="87"/>
+      <c r="P10" s="87"/>
+      <c r="Q10" s="87"/>
+      <c r="R10" s="87"/>
       <c r="S10" s="8"/>
     </row>
-    <row r="12" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D12" s="85" t="s">
+    <row r="12" spans="1:19" ht="15.9" x14ac:dyDescent="0.3">
+      <c r="D12" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="85"/>
-      <c r="F12" s="85"/>
-      <c r="G12" s="85"/>
-      <c r="H12" s="85"/>
-      <c r="I12" s="85"/>
-      <c r="J12" s="86" t="s">
+      <c r="E12" s="88"/>
+      <c r="F12" s="88"/>
+      <c r="G12" s="88"/>
+      <c r="H12" s="88"/>
+      <c r="I12" s="88"/>
+      <c r="J12" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="86"/>
-      <c r="L12" s="86"/>
-      <c r="M12" s="86"/>
-      <c r="N12" s="86"/>
-      <c r="O12" s="86"/>
-      <c r="P12" s="86"/>
-      <c r="Q12" s="86"/>
-      <c r="R12" s="86"/>
+      <c r="K12" s="89"/>
+      <c r="L12" s="89"/>
+      <c r="M12" s="89"/>
+      <c r="N12" s="89"/>
+      <c r="O12" s="89"/>
+      <c r="P12" s="89"/>
+      <c r="Q12" s="89"/>
+      <c r="R12" s="89"/>
       <c r="S12" s="9"/>
     </row>
-    <row r="13" spans="1:19" s="14" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="76" t="s">
+    <row r="13" spans="1:19" s="14" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="79" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="76"/>
-      <c r="C13" s="76"/>
+      <c r="B13" s="79"/>
+      <c r="C13" s="79"/>
       <c r="D13" s="46" t="s">
         <v>55</v>
       </c>
@@ -1521,11 +1523,11 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" s="77" t="s">
+      <c r="A14" s="80" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="78"/>
-      <c r="C14" s="79"/>
+      <c r="B14" s="81"/>
+      <c r="C14" s="82"/>
       <c r="D14" s="15">
         <v>0</v>
       </c>
@@ -1580,11 +1582,11 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" s="77" t="s">
+      <c r="A15" s="80" t="s">
         <v>82</v>
       </c>
-      <c r="B15" s="78"/>
-      <c r="C15" s="79"/>
+      <c r="B15" s="81"/>
+      <c r="C15" s="82"/>
       <c r="D15" s="15">
         <v>0</v>
       </c>
@@ -1639,33 +1641,33 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" s="77" t="s">
+      <c r="A16" s="80" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="78"/>
-      <c r="C16" s="79"/>
+      <c r="B16" s="81"/>
+      <c r="C16" s="82"/>
       <c r="D16" s="15">
         <v>0</v>
       </c>
       <c r="E16" s="15">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F16" s="15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G16" s="15">
         <v>0</v>
       </c>
       <c r="H16" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I16" s="16">
         <f t="shared" ref="I16:I22" si="3">+SUM(D16:H16)</f>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="J16" s="17">
-        <f t="shared" si="1"/>
-        <v>11000</v>
+        <f xml:space="preserve"> I16*1800</f>
+        <v>19800</v>
       </c>
       <c r="K16" s="17">
         <v>8000</v>
@@ -1681,16 +1683,16 @@
       </c>
       <c r="O16" s="18">
         <f t="shared" si="0"/>
-        <v>4750</v>
+        <v>6950</v>
       </c>
       <c r="P16" s="17"/>
       <c r="Q16" s="17">
-        <f t="shared" ref="Q16:R22" si="4">+J16+K16+L16+M16+O16+P16</f>
-        <v>30750</v>
+        <f t="shared" ref="Q16:Q22" si="4">+J16+K16+L16+M16+O16+P16</f>
+        <v>41750</v>
       </c>
       <c r="R16" s="17">
         <f>Q16*O5</f>
-        <v>30750</v>
+        <v>41750</v>
       </c>
       <c r="S16" s="18">
         <f t="shared" ref="S16:S22" si="5">+Q16-R16</f>
@@ -1698,11 +1700,11 @@
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A17" s="77" t="s">
+      <c r="A17" s="80" t="s">
         <v>83</v>
       </c>
-      <c r="B17" s="78"/>
-      <c r="C17" s="79"/>
+      <c r="B17" s="81"/>
+      <c r="C17" s="82"/>
       <c r="D17" s="15">
         <v>0</v>
       </c>
@@ -1755,22 +1757,22 @@
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A18" s="77" t="s">
+      <c r="A18" s="80" t="s">
         <v>84</v>
       </c>
-      <c r="B18" s="78"/>
-      <c r="C18" s="79"/>
+      <c r="B18" s="81"/>
+      <c r="C18" s="82"/>
       <c r="D18" s="15">
         <v>0</v>
       </c>
       <c r="E18" s="15">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F18" s="15">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G18" s="15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H18" s="15">
         <v>1</v>
@@ -1780,8 +1782,8 @@
         <v>12</v>
       </c>
       <c r="J18" s="17">
-        <f t="shared" si="1"/>
-        <v>26400</v>
+        <f xml:space="preserve"> I18*1800</f>
+        <v>21600</v>
       </c>
       <c r="K18" s="17">
         <v>23750</v>
@@ -1797,16 +1799,16 @@
       </c>
       <c r="O18" s="18">
         <f t="shared" si="0"/>
-        <v>12537.5</v>
+        <v>11337.5</v>
       </c>
       <c r="P18" s="17"/>
       <c r="Q18" s="17">
         <f t="shared" si="4"/>
-        <v>62687.5</v>
+        <v>56687.5</v>
       </c>
       <c r="R18" s="17">
         <f>Q18*O5</f>
-        <v>62687.5</v>
+        <v>56687.5</v>
       </c>
       <c r="S18" s="18">
         <f t="shared" si="5"/>
@@ -1814,11 +1816,11 @@
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A19" s="77" t="s">
+      <c r="A19" s="80" t="s">
         <v>85</v>
       </c>
-      <c r="B19" s="78"/>
-      <c r="C19" s="79"/>
+      <c r="B19" s="81"/>
+      <c r="C19" s="82"/>
       <c r="D19" s="15">
         <v>0</v>
       </c>
@@ -1839,8 +1841,8 @@
         <v>6</v>
       </c>
       <c r="J19" s="17">
-        <f t="shared" si="1"/>
-        <v>13200</v>
+        <f xml:space="preserve"> I19*1800</f>
+        <v>10800</v>
       </c>
       <c r="K19" s="17">
         <v>30000</v>
@@ -1856,16 +1858,16 @@
       </c>
       <c r="O19" s="18">
         <f t="shared" si="0"/>
-        <v>10800</v>
+        <v>10200</v>
       </c>
       <c r="P19" s="17"/>
       <c r="Q19" s="17">
         <f t="shared" si="4"/>
-        <v>54000</v>
+        <v>51000</v>
       </c>
       <c r="R19" s="17">
         <f>Q19*O5</f>
-        <v>54000</v>
+        <v>51000</v>
       </c>
       <c r="S19" s="18">
         <f t="shared" si="5"/>
@@ -1873,11 +1875,11 @@
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A20" s="77" t="s">
+      <c r="A20" s="80" t="s">
         <v>86</v>
       </c>
-      <c r="B20" s="78"/>
-      <c r="C20" s="79"/>
+      <c r="B20" s="81"/>
+      <c r="C20" s="82"/>
       <c r="D20" s="15">
         <v>0</v>
       </c>
@@ -1898,8 +1900,8 @@
         <v>5</v>
       </c>
       <c r="J20" s="17">
-        <f t="shared" si="1"/>
-        <v>11000</v>
+        <f xml:space="preserve"> I20*1800</f>
+        <v>9000</v>
       </c>
       <c r="K20" s="17">
         <v>800</v>
@@ -1915,16 +1917,16 @@
       </c>
       <c r="O20" s="18">
         <f t="shared" si="0"/>
-        <v>2950</v>
+        <v>2450</v>
       </c>
       <c r="P20" s="17"/>
       <c r="Q20" s="17">
         <f t="shared" si="4"/>
-        <v>14750</v>
+        <v>12250</v>
       </c>
       <c r="R20" s="17">
         <f>Q20*O5</f>
-        <v>14750</v>
+        <v>12250</v>
       </c>
       <c r="S20" s="18">
         <f t="shared" si="5"/>
@@ -1932,11 +1934,11 @@
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A21" s="77" t="s">
+      <c r="A21" s="80" t="s">
         <v>87</v>
       </c>
-      <c r="B21" s="78"/>
-      <c r="C21" s="79"/>
+      <c r="B21" s="81"/>
+      <c r="C21" s="82"/>
       <c r="D21" s="15">
         <v>0</v>
       </c>
@@ -1989,11 +1991,11 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A22" s="77" t="s">
+      <c r="A22" s="80" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="78"/>
-      <c r="C22" s="79"/>
+      <c r="B22" s="81"/>
+      <c r="C22" s="82"/>
       <c r="D22" s="15">
         <v>0</v>
       </c>
@@ -2046,38 +2048,38 @@
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A23" s="73" t="s">
+      <c r="A23" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="73"/>
-      <c r="C23" s="73"/>
+      <c r="B23" s="76"/>
+      <c r="C23" s="76"/>
       <c r="D23" s="15">
         <f t="shared" ref="D23:S23" si="6">SUM(D14:D22)</f>
         <v>0</v>
       </c>
       <c r="E23" s="15">
         <f t="shared" si="6"/>
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="F23" s="15">
         <f t="shared" si="6"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G23" s="15">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H23" s="15">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I23" s="19">
         <f t="shared" si="6"/>
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J23" s="20">
         <f t="shared" si="6"/>
-        <v>61600</v>
+        <v>61200</v>
       </c>
       <c r="K23" s="20">
         <f t="shared" si="6"/>
@@ -2097,7 +2099,7 @@
       </c>
       <c r="O23" s="20">
         <f t="shared" si="6"/>
-        <v>31037.5</v>
+        <v>30937.5</v>
       </c>
       <c r="P23" s="20">
         <f t="shared" si="6"/>
@@ -2105,11 +2107,11 @@
       </c>
       <c r="Q23" s="20">
         <f t="shared" si="6"/>
-        <v>164187.5</v>
+        <v>163687.5</v>
       </c>
       <c r="R23" s="21">
         <f t="shared" si="6"/>
-        <v>164187.5</v>
+        <v>163687.5</v>
       </c>
       <c r="S23" s="22">
         <f t="shared" si="6"/>
@@ -2128,7 +2130,7 @@
       <c r="H24" s="25"/>
       <c r="I24" s="25"/>
       <c r="J24" s="23"/>
-      <c r="K24" s="90" t="s">
+      <c r="K24" s="62" t="s">
         <v>94</v>
       </c>
       <c r="L24" s="23"/>
@@ -2137,7 +2139,7 @@
       <c r="O24" s="23"/>
       <c r="P24" s="23"/>
       <c r="Q24" s="23"/>
-      <c r="R24" s="90" t="s">
+      <c r="R24" s="62" t="s">
         <v>95</v>
       </c>
       <c r="S24" s="23"/>
@@ -2157,7 +2159,7 @@
       <c r="I25" s="29"/>
       <c r="J25" s="20">
         <f>IF(I23=0,0,(J23/I23))</f>
-        <v>2200</v>
+        <v>1800</v>
       </c>
       <c r="K25" s="23"/>
       <c r="L25" s="23"/>
@@ -2175,24 +2177,24 @@
       <c r="S26" s="31"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A27" s="72" t="s">
+      <c r="A27" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="72"/>
-      <c r="C27" s="72"/>
-      <c r="D27" s="72"/>
-      <c r="E27" s="72"/>
-      <c r="F27" s="72"/>
-      <c r="G27" s="72"/>
-      <c r="H27" s="72"/>
-      <c r="I27" s="72"/>
-      <c r="J27" s="72"/>
-      <c r="K27" s="72"/>
-      <c r="L27" s="72"/>
-      <c r="M27" s="72"/>
-      <c r="N27" s="72"/>
-      <c r="O27" s="72"/>
-      <c r="P27" s="72"/>
+      <c r="B27" s="75"/>
+      <c r="C27" s="75"/>
+      <c r="D27" s="75"/>
+      <c r="E27" s="75"/>
+      <c r="F27" s="75"/>
+      <c r="G27" s="75"/>
+      <c r="H27" s="75"/>
+      <c r="I27" s="75"/>
+      <c r="J27" s="75"/>
+      <c r="K27" s="75"/>
+      <c r="L27" s="75"/>
+      <c r="M27" s="75"/>
+      <c r="N27" s="75"/>
+      <c r="O27" s="75"/>
+      <c r="P27" s="75"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="32"/>
@@ -2212,7 +2214,7 @@
       <c r="O28" s="32"/>
       <c r="P28" s="32"/>
     </row>
-    <row r="29" spans="1:20" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" ht="41.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="32" t="s">
         <v>31</v>
       </c>
@@ -2232,104 +2234,104 @@
       <c r="O29" s="32"/>
       <c r="P29" s="32"/>
     </row>
-    <row r="30" spans="1:20" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="64" t="str">
+    <row r="30" spans="1:20" ht="41.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="67" t="str">
         <f>CONCATENATE("participant"," ",J6)</f>
         <v>participant VIZLORE</v>
       </c>
-      <c r="B30" s="65"/>
+      <c r="B30" s="68"/>
       <c r="C30" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="74" t="s">
+      <c r="D30" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="E30" s="75"/>
-      <c r="F30" s="75"/>
-      <c r="G30" s="75"/>
-      <c r="H30" s="75"/>
-      <c r="I30" s="75"/>
-      <c r="J30" s="75"/>
-      <c r="K30" s="75"/>
-      <c r="L30" s="75"/>
-      <c r="M30" s="75"/>
-      <c r="N30" s="75"/>
-      <c r="O30" s="75"/>
-      <c r="P30" s="75"/>
+      <c r="E30" s="78"/>
+      <c r="F30" s="78"/>
+      <c r="G30" s="78"/>
+      <c r="H30" s="78"/>
+      <c r="I30" s="78"/>
+      <c r="J30" s="78"/>
+      <c r="K30" s="78"/>
+      <c r="L30" s="78"/>
+      <c r="M30" s="78"/>
+      <c r="N30" s="78"/>
+      <c r="O30" s="78"/>
+      <c r="P30" s="78"/>
     </row>
     <row r="31" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="61" t="s">
+      <c r="A31" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="61"/>
-      <c r="C31" s="89" t="s">
+      <c r="B31" s="64"/>
+      <c r="C31" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="D31" s="68" t="s">
+      <c r="D31" s="71" t="s">
         <v>89</v>
       </c>
-      <c r="E31" s="63"/>
-      <c r="F31" s="63"/>
-      <c r="G31" s="63"/>
-      <c r="H31" s="63"/>
-      <c r="I31" s="63"/>
-      <c r="J31" s="63"/>
-      <c r="K31" s="63"/>
-      <c r="L31" s="63"/>
-      <c r="M31" s="63"/>
-      <c r="N31" s="63"/>
-      <c r="O31" s="63"/>
-      <c r="P31" s="63"/>
+      <c r="E31" s="66"/>
+      <c r="F31" s="66"/>
+      <c r="G31" s="66"/>
+      <c r="H31" s="66"/>
+      <c r="I31" s="66"/>
+      <c r="J31" s="66"/>
+      <c r="K31" s="66"/>
+      <c r="L31" s="66"/>
+      <c r="M31" s="66"/>
+      <c r="N31" s="66"/>
+      <c r="O31" s="66"/>
+      <c r="P31" s="66"/>
       <c r="S31" s="31"/>
     </row>
-    <row r="32" spans="1:20" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="61" t="s">
+    <row r="32" spans="1:20" ht="29.3" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="61"/>
+      <c r="B32" s="64"/>
       <c r="C32" s="34">
         <v>62550</v>
       </c>
-      <c r="D32" s="63" t="s">
+      <c r="D32" s="66" t="s">
         <v>90</v>
       </c>
-      <c r="E32" s="63"/>
-      <c r="F32" s="63"/>
-      <c r="G32" s="63"/>
-      <c r="H32" s="63"/>
-      <c r="I32" s="63"/>
-      <c r="J32" s="63"/>
-      <c r="K32" s="63"/>
-      <c r="L32" s="63"/>
-      <c r="M32" s="63"/>
-      <c r="N32" s="63"/>
-      <c r="O32" s="63"/>
-      <c r="P32" s="63"/>
+      <c r="E32" s="66"/>
+      <c r="F32" s="66"/>
+      <c r="G32" s="66"/>
+      <c r="H32" s="66"/>
+      <c r="I32" s="66"/>
+      <c r="J32" s="66"/>
+      <c r="K32" s="66"/>
+      <c r="L32" s="66"/>
+      <c r="M32" s="66"/>
+      <c r="N32" s="66"/>
+      <c r="O32" s="66"/>
+      <c r="P32" s="66"/>
       <c r="S32" s="31"/>
     </row>
-    <row r="33" spans="1:19" ht="31.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="61" t="s">
+    <row r="33" spans="1:19" ht="31.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="61"/>
+      <c r="B33" s="64"/>
       <c r="C33" s="34">
         <v>40000</v>
       </c>
-      <c r="D33" s="63" t="s">
+      <c r="D33" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="E33" s="63"/>
-      <c r="F33" s="63"/>
-      <c r="G33" s="63"/>
-      <c r="H33" s="63"/>
-      <c r="I33" s="63"/>
-      <c r="J33" s="63"/>
-      <c r="K33" s="63"/>
-      <c r="L33" s="63"/>
-      <c r="M33" s="63"/>
-      <c r="N33" s="63"/>
-      <c r="O33" s="63"/>
-      <c r="P33" s="63"/>
+      <c r="E33" s="66"/>
+      <c r="F33" s="66"/>
+      <c r="G33" s="66"/>
+      <c r="H33" s="66"/>
+      <c r="I33" s="66"/>
+      <c r="J33" s="66"/>
+      <c r="K33" s="66"/>
+      <c r="L33" s="66"/>
+      <c r="M33" s="66"/>
+      <c r="N33" s="66"/>
+      <c r="O33" s="66"/>
+      <c r="P33" s="66"/>
       <c r="S33" s="31"/>
     </row>
     <row r="34" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.3">
@@ -2363,99 +2365,99 @@
       <c r="P35" s="37"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A36" s="64" t="str">
+      <c r="A36" s="67" t="str">
         <f>CONCATENATE("participant"," ",C9)</f>
         <v xml:space="preserve">participant </v>
       </c>
-      <c r="B36" s="65"/>
+      <c r="B36" s="68"/>
       <c r="C36" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D36" s="66" t="s">
+      <c r="D36" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="E36" s="67"/>
-      <c r="F36" s="67"/>
-      <c r="G36" s="67"/>
-      <c r="H36" s="67"/>
-      <c r="I36" s="67"/>
-      <c r="J36" s="67"/>
-      <c r="K36" s="67"/>
-      <c r="L36" s="67"/>
-      <c r="M36" s="67"/>
-      <c r="N36" s="67"/>
-      <c r="O36" s="67"/>
-      <c r="P36" s="67"/>
-    </row>
-    <row r="37" spans="1:19" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="61" t="s">
+      <c r="E36" s="70"/>
+      <c r="F36" s="70"/>
+      <c r="G36" s="70"/>
+      <c r="H36" s="70"/>
+      <c r="I36" s="70"/>
+      <c r="J36" s="70"/>
+      <c r="K36" s="70"/>
+      <c r="L36" s="70"/>
+      <c r="M36" s="70"/>
+      <c r="N36" s="70"/>
+      <c r="O36" s="70"/>
+      <c r="P36" s="70"/>
+    </row>
+    <row r="37" spans="1:19" ht="27.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="61"/>
+      <c r="B37" s="64"/>
       <c r="C37" s="34">
         <v>9000</v>
       </c>
-      <c r="D37" s="62" t="s">
+      <c r="D37" s="65" t="s">
         <v>93</v>
       </c>
-      <c r="E37" s="63"/>
-      <c r="F37" s="63"/>
-      <c r="G37" s="63"/>
-      <c r="H37" s="63"/>
-      <c r="I37" s="63"/>
-      <c r="J37" s="63"/>
-      <c r="K37" s="63"/>
-      <c r="L37" s="63"/>
-      <c r="M37" s="63"/>
-      <c r="N37" s="63"/>
-      <c r="O37" s="63"/>
-      <c r="P37" s="63"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="66"/>
+      <c r="G37" s="66"/>
+      <c r="H37" s="66"/>
+      <c r="I37" s="66"/>
+      <c r="J37" s="66"/>
+      <c r="K37" s="66"/>
+      <c r="L37" s="66"/>
+      <c r="M37" s="66"/>
+      <c r="N37" s="66"/>
+      <c r="O37" s="66"/>
+      <c r="P37" s="66"/>
       <c r="S37" s="31"/>
     </row>
     <row r="38" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="61" t="s">
+      <c r="A38" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="61"/>
+      <c r="B38" s="64"/>
       <c r="C38" s="34">
         <v>0</v>
       </c>
-      <c r="D38" s="69"/>
-      <c r="E38" s="70"/>
-      <c r="F38" s="70"/>
-      <c r="G38" s="70"/>
-      <c r="H38" s="70"/>
-      <c r="I38" s="70"/>
-      <c r="J38" s="70"/>
-      <c r="K38" s="70"/>
-      <c r="L38" s="70"/>
-      <c r="M38" s="70"/>
-      <c r="N38" s="70"/>
-      <c r="O38" s="70"/>
-      <c r="P38" s="71"/>
+      <c r="D38" s="72"/>
+      <c r="E38" s="73"/>
+      <c r="F38" s="73"/>
+      <c r="G38" s="73"/>
+      <c r="H38" s="73"/>
+      <c r="I38" s="73"/>
+      <c r="J38" s="73"/>
+      <c r="K38" s="73"/>
+      <c r="L38" s="73"/>
+      <c r="M38" s="73"/>
+      <c r="N38" s="73"/>
+      <c r="O38" s="73"/>
+      <c r="P38" s="74"/>
       <c r="S38" s="31"/>
     </row>
     <row r="39" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="61" t="s">
+      <c r="A39" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="61"/>
+      <c r="B39" s="64"/>
       <c r="C39" s="34">
         <v>0</v>
       </c>
-      <c r="D39" s="62"/>
-      <c r="E39" s="63"/>
-      <c r="F39" s="63"/>
-      <c r="G39" s="63"/>
-      <c r="H39" s="63"/>
-      <c r="I39" s="63"/>
-      <c r="J39" s="63"/>
-      <c r="K39" s="63"/>
-      <c r="L39" s="63"/>
-      <c r="M39" s="63"/>
-      <c r="N39" s="63"/>
-      <c r="O39" s="63"/>
-      <c r="P39" s="63"/>
+      <c r="D39" s="65"/>
+      <c r="E39" s="66"/>
+      <c r="F39" s="66"/>
+      <c r="G39" s="66"/>
+      <c r="H39" s="66"/>
+      <c r="I39" s="66"/>
+      <c r="J39" s="66"/>
+      <c r="K39" s="66"/>
+      <c r="L39" s="66"/>
+      <c r="M39" s="66"/>
+      <c r="N39" s="66"/>
+      <c r="O39" s="66"/>
+      <c r="P39" s="66"/>
       <c r="S39" s="31"/>
     </row>
   </sheetData>
@@ -2527,10 +2529,10 @@
   <dimension ref="A1:P46"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.65" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.77734375" customWidth="1"/>
     <col min="3" max="3" width="11.5546875" customWidth="1"/>
@@ -2539,18 +2541,18 @@
     <col min="7" max="7" width="17.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="87" t="s">
+    <row r="1" spans="1:16" ht="15.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:16" ht="18.95" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="90" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="88"/>
+      <c r="C2" s="91"/>
       <c r="D2" s="42">
         <f>SUM(P5:P33)</f>
-        <v>30750</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="162.6" x14ac:dyDescent="0.3">
+        <v>27240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="156.19999999999999" x14ac:dyDescent="0.3">
       <c r="B4" s="57" t="s">
         <v>48</v>
       </c>
@@ -2597,262 +2599,311 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
       <c r="A5" s="60"/>
-      <c r="B5" s="55" t="s">
-        <v>58</v>
+      <c r="B5" s="63" t="s">
+        <v>96</v>
       </c>
       <c r="C5" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="55" t="s">
+      <c r="D5" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="55" t="s">
+      <c r="E5" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="F5" s="55" t="s">
+      <c r="F5" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="G5" s="55" t="s">
-        <v>67</v>
-      </c>
-      <c r="H5" s="55"/>
-      <c r="I5" s="55"/>
-      <c r="J5" s="55">
-        <v>3</v>
-      </c>
-      <c r="K5" s="55"/>
-      <c r="L5" s="55"/>
-      <c r="M5" s="55">
+      <c r="G5" s="63" t="s">
+        <v>97</v>
+      </c>
+      <c r="H5" s="63">
+        <v>1</v>
+      </c>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63">
+        <v>1</v>
+      </c>
+      <c r="K5" s="63"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="63">
         <v>4</v>
       </c>
-      <c r="N5" s="55">
-        <v>2400</v>
-      </c>
-      <c r="O5" s="55">
-        <v>2250</v>
-      </c>
-      <c r="P5" s="55">
-        <v>6650</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="N5" s="63">
+        <v>1260</v>
+      </c>
+      <c r="O5" s="63">
+        <v>880</v>
+      </c>
+      <c r="P5" s="63">
+        <f>N5+O5</f>
+        <v>2140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
       <c r="A6" s="58"/>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="63" t="s">
         <v>58</v>
       </c>
       <c r="C6" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="D6" s="55" t="s">
+      <c r="D6" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="55" t="s">
+      <c r="E6" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="F6" s="55" t="s">
+      <c r="F6" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="55" t="s">
+      <c r="G6" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55">
+      <c r="H6" s="63"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63">
         <v>3</v>
       </c>
-      <c r="K6" s="55"/>
-      <c r="L6" s="55"/>
-      <c r="M6" s="55">
+      <c r="K6" s="63"/>
+      <c r="L6" s="63"/>
+      <c r="M6" s="63">
         <v>4</v>
       </c>
-      <c r="N6" s="55">
-        <v>2400</v>
-      </c>
-      <c r="O6" s="55">
-        <v>2250</v>
-      </c>
-      <c r="P6" s="55">
-        <v>6650</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="N6" s="63">
+        <v>1890</v>
+      </c>
+      <c r="O6" s="63">
+        <v>1320</v>
+      </c>
+      <c r="P6" s="63">
+        <v>3210</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
       <c r="A7" s="58"/>
-      <c r="B7" s="55" t="s">
+      <c r="B7" s="63" t="s">
         <v>58</v>
       </c>
       <c r="C7" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="D7" s="55" t="s">
+      <c r="D7" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="55" t="s">
+      <c r="E7" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="55" t="s">
+      <c r="F7" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="55" t="s">
+      <c r="G7" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55">
+      <c r="H7" s="63"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="63">
         <v>3</v>
       </c>
-      <c r="K7" s="55"/>
-      <c r="L7" s="55"/>
-      <c r="M7" s="55">
+      <c r="K7" s="63"/>
+      <c r="L7" s="63"/>
+      <c r="M7" s="63">
         <v>4</v>
       </c>
-      <c r="N7" s="55">
-        <v>2400</v>
-      </c>
-      <c r="O7" s="55">
-        <v>2250</v>
-      </c>
-      <c r="P7" s="55">
-        <v>6650</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="N7" s="63">
+        <v>1890</v>
+      </c>
+      <c r="O7" s="63">
+        <v>1320</v>
+      </c>
+      <c r="P7" s="63">
+        <v>3210</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
       <c r="A8" s="58"/>
-      <c r="B8" s="55" t="s">
-        <v>76</v>
+      <c r="B8" s="63" t="s">
+        <v>58</v>
       </c>
       <c r="C8" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="D8" s="55" t="s">
+      <c r="D8" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="E8" s="55" t="s">
+      <c r="E8" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="F8" s="55" t="s">
+      <c r="F8" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="G8" s="55" t="s">
-        <v>68</v>
-      </c>
-      <c r="H8" s="55"/>
-      <c r="I8" s="55"/>
-      <c r="J8" s="55">
-        <v>2</v>
-      </c>
-      <c r="K8" s="55"/>
-      <c r="L8" s="55"/>
-      <c r="M8" s="55">
+      <c r="G8" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" s="63"/>
+      <c r="I8" s="63"/>
+      <c r="J8" s="63">
+        <v>3</v>
+      </c>
+      <c r="K8" s="63"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="63">
         <v>4</v>
       </c>
-      <c r="N8" s="55">
-        <v>2000</v>
-      </c>
-      <c r="O8" s="55">
-        <v>1400</v>
-      </c>
-      <c r="P8" s="55">
-        <v>5100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N8" s="63">
+        <v>1890</v>
+      </c>
+      <c r="O8" s="63">
+        <v>1320</v>
+      </c>
+      <c r="P8" s="63">
+        <v>3210</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="59"/>
-      <c r="B9" s="55" t="s">
-        <v>59</v>
+      <c r="B9" s="63" t="s">
+        <v>58</v>
       </c>
       <c r="C9" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="D9" s="55" t="s">
+      <c r="D9" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="55" t="s">
+      <c r="E9" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="F9" s="55" t="s">
+      <c r="F9" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="G9" s="55" t="s">
+      <c r="G9" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" s="63"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="63">
+        <v>3</v>
+      </c>
+      <c r="K9" s="63"/>
+      <c r="L9" s="63"/>
+      <c r="M9" s="63">
+        <v>4</v>
+      </c>
+      <c r="N9" s="63">
+        <v>1890</v>
+      </c>
+      <c r="O9" s="63">
+        <v>1320</v>
+      </c>
+      <c r="P9" s="63">
+        <v>3210</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
+      <c r="A10" s="55"/>
+      <c r="B10" s="63" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="58" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="63" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="63" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="63" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" s="63" t="s">
+        <v>68</v>
+      </c>
+      <c r="H10" s="63"/>
+      <c r="I10" s="63"/>
+      <c r="J10" s="63">
+        <v>3</v>
+      </c>
+      <c r="K10" s="63"/>
+      <c r="L10" s="63">
+        <v>2</v>
+      </c>
+      <c r="M10" s="63">
+        <v>4</v>
+      </c>
+      <c r="N10" s="63">
+        <v>6250</v>
+      </c>
+      <c r="O10" s="63">
+        <v>2200</v>
+      </c>
+      <c r="P10" s="63">
+        <v>8450</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
+      <c r="A11" s="55"/>
+      <c r="B11" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="58" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="63" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="63" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="63" t="s">
+        <v>66</v>
+      </c>
+      <c r="G11" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="H9" s="55"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="55">
+      <c r="H11" s="63"/>
+      <c r="I11" s="63"/>
+      <c r="J11" s="63">
         <v>3</v>
       </c>
-      <c r="K9" s="55"/>
-      <c r="L9" s="55"/>
-      <c r="M9" s="55">
+      <c r="K11" s="63"/>
+      <c r="L11" s="63"/>
+      <c r="M11" s="63">
         <v>5</v>
       </c>
-      <c r="N9" s="55">
-        <v>3000</v>
-      </c>
-      <c r="O9" s="55">
-        <v>2700</v>
-      </c>
-      <c r="P9" s="55">
-        <f t="shared" ref="P9" si="0">N9+O9</f>
-        <v>5700</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="55"/>
-      <c r="B10" s="55"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="55"/>
-      <c r="J10" s="55"/>
-      <c r="K10" s="55"/>
-      <c r="L10" s="55"/>
-      <c r="M10" s="55"/>
-      <c r="N10" s="55"/>
-      <c r="O10" s="55"/>
-      <c r="P10" s="55"/>
-    </row>
-    <row r="11" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="55"/>
-      <c r="B11" s="55"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="38"/>
-      <c r="L11" s="38"/>
-      <c r="M11" s="38"/>
-      <c r="N11" s="38"/>
-      <c r="O11" s="38"/>
-      <c r="P11" s="38"/>
-    </row>
-    <row r="12" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="N11" s="63">
+        <v>1890</v>
+      </c>
+      <c r="O11" s="63">
+        <v>1920</v>
+      </c>
+      <c r="P11" s="63">
+        <f t="shared" ref="P11" si="0">N11+O11</f>
+        <v>3810</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
       <c r="A12" s="55"/>
-      <c r="B12" s="55"/>
+      <c r="B12" s="63"/>
       <c r="C12" s="58"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="38"/>
-      <c r="N12" s="38"/>
-      <c r="O12" s="38"/>
-      <c r="P12" s="38"/>
-    </row>
-    <row r="13" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D12" s="63"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="63"/>
+      <c r="H12" s="63"/>
+      <c r="I12" s="63"/>
+      <c r="J12" s="63"/>
+      <c r="K12" s="63"/>
+      <c r="L12" s="63"/>
+      <c r="M12" s="63"/>
+      <c r="N12" s="63"/>
+      <c r="O12" s="63"/>
+      <c r="P12" s="63"/>
+    </row>
+    <row r="13" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
       <c r="A13" s="55"/>
       <c r="B13" s="55"/>
       <c r="C13" s="58"/>
@@ -2870,7 +2921,7 @@
       <c r="O13" s="38"/>
       <c r="P13" s="38"/>
     </row>
-    <row r="14" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
       <c r="A14" s="55"/>
       <c r="B14" s="55"/>
       <c r="C14" s="58"/>
@@ -2888,7 +2939,7 @@
       <c r="O14" s="38"/>
       <c r="P14" s="38"/>
     </row>
-    <row r="15" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
       <c r="A15" s="55"/>
       <c r="B15" s="55"/>
       <c r="C15" s="59"/>
@@ -2906,7 +2957,7 @@
       <c r="O15" s="48"/>
       <c r="P15" s="38"/>
     </row>
-    <row r="16" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
       <c r="A16" s="55"/>
       <c r="B16" s="55"/>
       <c r="C16" s="58"/>
@@ -2924,7 +2975,7 @@
       <c r="O16" s="48"/>
       <c r="P16" s="38"/>
     </row>
-    <row r="17" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
       <c r="A17" s="55"/>
       <c r="B17" s="55"/>
       <c r="C17" s="58"/>
@@ -2942,7 +2993,7 @@
       <c r="O17" s="48"/>
       <c r="P17" s="38"/>
     </row>
-    <row r="18" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
       <c r="A18" s="55"/>
       <c r="B18" s="55"/>
       <c r="C18" s="59"/>
@@ -2960,7 +3011,7 @@
       <c r="O18" s="48"/>
       <c r="P18" s="38"/>
     </row>
-    <row r="19" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
       <c r="A19" s="55"/>
       <c r="B19" s="55"/>
       <c r="C19" s="58"/>
@@ -2978,7 +3029,7 @@
       <c r="O19" s="38"/>
       <c r="P19" s="38"/>
     </row>
-    <row r="20" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
       <c r="A20" s="55"/>
       <c r="B20" s="55"/>
       <c r="C20" s="58"/>
@@ -2996,7 +3047,7 @@
       <c r="O20" s="48"/>
       <c r="P20" s="38"/>
     </row>
-    <row r="21" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
       <c r="A21" s="55"/>
       <c r="B21" s="55"/>
       <c r="C21" s="58"/>
@@ -3014,7 +3065,7 @@
       <c r="O21" s="48"/>
       <c r="P21" s="38"/>
     </row>
-    <row r="22" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
       <c r="A22" s="55"/>
       <c r="B22" s="55"/>
       <c r="C22" s="59"/>
@@ -3032,7 +3083,7 @@
       <c r="O22" s="48"/>
       <c r="P22" s="38"/>
     </row>
-    <row r="23" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
       <c r="A23" s="55"/>
       <c r="B23" s="55"/>
       <c r="C23" s="58"/>
@@ -3050,7 +3101,7 @@
       <c r="O23" s="48"/>
       <c r="P23" s="48"/>
     </row>
-    <row r="24" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
       <c r="A24" s="55"/>
       <c r="B24" s="55"/>
       <c r="C24" s="58"/>
@@ -3068,7 +3119,7 @@
       <c r="O24" s="48"/>
       <c r="P24" s="48"/>
     </row>
-    <row r="25" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
       <c r="A25" s="55"/>
       <c r="B25" s="55"/>
       <c r="C25" s="58"/>
@@ -3086,7 +3137,7 @@
       <c r="O25" s="48"/>
       <c r="P25" s="48"/>
     </row>
-    <row r="26" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
       <c r="A26" s="55"/>
       <c r="B26" s="55"/>
       <c r="C26" s="59"/>
@@ -3104,7 +3155,7 @@
       <c r="O26" s="48"/>
       <c r="P26" s="48"/>
     </row>
-    <row r="27" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
       <c r="A27" s="55"/>
       <c r="B27" s="55"/>
       <c r="C27" s="58"/>
@@ -3122,7 +3173,7 @@
       <c r="O27" s="48"/>
       <c r="P27" s="38"/>
     </row>
-    <row r="28" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
       <c r="A28" s="55"/>
       <c r="B28" s="55"/>
       <c r="C28" s="58"/>
@@ -3140,7 +3191,7 @@
       <c r="O28" s="48"/>
       <c r="P28" s="38"/>
     </row>
-    <row r="29" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
       <c r="A29" s="55"/>
       <c r="B29" s="55"/>
       <c r="C29" s="58"/>
@@ -3158,7 +3209,7 @@
       <c r="O29" s="48"/>
       <c r="P29" s="38"/>
     </row>
-    <row r="30" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
       <c r="A30" s="55"/>
       <c r="B30" s="55"/>
       <c r="C30" s="59"/>
@@ -3176,7 +3227,7 @@
       <c r="O30" s="48"/>
       <c r="P30" s="38"/>
     </row>
-    <row r="31" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
       <c r="A31" s="55"/>
       <c r="B31" s="55"/>
       <c r="C31" s="59"/>
@@ -3194,7 +3245,7 @@
       <c r="O31" s="38"/>
       <c r="P31" s="38"/>
     </row>
-    <row r="32" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
       <c r="A32" s="55"/>
       <c r="B32" s="55"/>
       <c r="C32" s="58"/>
@@ -3212,7 +3263,7 @@
       <c r="O32" s="38"/>
       <c r="P32" s="38"/>
     </row>
-    <row r="33" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
       <c r="A33" s="55"/>
       <c r="B33" s="55"/>
       <c r="C33" s="58"/>
@@ -3230,7 +3281,7 @@
       <c r="O33" s="38"/>
       <c r="P33" s="38"/>
     </row>
-    <row r="34" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
       <c r="A34" s="55"/>
       <c r="B34" s="55"/>
       <c r="C34" s="58"/>
@@ -3248,7 +3299,7 @@
       <c r="O34" s="48"/>
       <c r="P34" s="48"/>
     </row>
-    <row r="35" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
       <c r="A35" s="55"/>
       <c r="B35" s="55"/>
       <c r="C35" s="59"/>
@@ -3284,7 +3335,7 @@
       <c r="O36" s="48"/>
       <c r="P36" s="48"/>
     </row>
-    <row r="37" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
       <c r="A37" s="55"/>
       <c r="B37" s="55"/>
       <c r="C37" s="59"/>
@@ -3302,7 +3353,7 @@
       <c r="O37" s="48"/>
       <c r="P37" s="48"/>
     </row>
-    <row r="38" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
       <c r="A38" s="55"/>
       <c r="B38" s="55"/>
       <c r="C38" s="58"/>
@@ -3320,7 +3371,7 @@
       <c r="O38" s="48"/>
       <c r="P38" s="48"/>
     </row>
-    <row r="39" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
       <c r="A39" s="55"/>
       <c r="B39" s="55"/>
       <c r="C39" s="58"/>
@@ -3338,7 +3389,7 @@
       <c r="O39" s="48"/>
       <c r="P39" s="48"/>
     </row>
-    <row r="40" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
       <c r="A40" s="55"/>
       <c r="B40" s="55"/>
       <c r="C40" s="59"/>
@@ -3374,7 +3425,7 @@
       <c r="O41" s="48"/>
       <c r="P41" s="48"/>
     </row>
-    <row r="42" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
       <c r="A42" s="55"/>
       <c r="B42" s="55"/>
       <c r="C42" s="58"/>
@@ -3478,10 +3529,10 @@
   <dimension ref="B1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8:I9"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.65" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18.5546875" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" customWidth="1"/>
@@ -3491,18 +3542,18 @@
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="87" t="s">
+    <row r="1" spans="2:9" ht="15.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:9" ht="18.95" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="90" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="88"/>
+      <c r="C2" s="91"/>
       <c r="D2" s="42">
         <f>SUM(I5:I35)</f>
         <v>62550</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" ht="43.95" x14ac:dyDescent="0.3">
       <c r="B4" s="40" t="s">
         <v>48</v>
       </c>
@@ -4028,7 +4079,7 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.65" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18.5546875" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
@@ -4037,18 +4088,18 @@
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="87" t="s">
+    <row r="1" spans="2:9" ht="15.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:9" ht="18.95" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="90" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="88"/>
+      <c r="C2" s="91"/>
       <c r="D2" s="42">
         <f>SUM(I5:I34)</f>
         <v>9000</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" ht="43.95" x14ac:dyDescent="0.3">
       <c r="B4" s="40" t="s">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
Pregledala sve i ubacila CV
</commit_message>
<xml_diff>
--- a/2b Format partner budget - Horizon2020  VIZLORE .xlsx
+++ b/2b Format partner budget - Horizon2020  VIZLORE .xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Anja\Fakultet\6. semestar\USP\Projekat\Projekat\Projekat_Faza1_ver1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D59F89CF-FBED-4DF9-ACD8-31CDB89ED95B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9189"/>
+    <workbookView xWindow="9564" yWindow="4788" windowWidth="17280" windowHeight="8964" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Detaljno budzet" sheetId="1" r:id="rId1"/>
@@ -15,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Travel - budzet'!$B$4:$P$46</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="96">
   <si>
     <t>Partner budget Horizon 2020</t>
   </si>
@@ -305,31 +311,25 @@
     <t>Sheet Equipment-budzet</t>
   </si>
   <si>
-    <t>30750</t>
-  </si>
-  <si>
     <t>Potrošni materijal, ketering, osnovni kancelarijski materijal, ugostiteljstvo, publikacije</t>
   </si>
   <si>
     <t>Sheet Subcontracting - budzet</t>
   </si>
   <si>
-    <t>eqipment</t>
-  </si>
-  <si>
-    <t>isto kao pored ako je reasearch</t>
-  </si>
-  <si>
     <t>WP1</t>
   </si>
   <si>
     <t>Athens</t>
+  </si>
+  <si>
+    <t>27240</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
@@ -822,53 +822,11 @@
     </xf>
     <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -879,7 +837,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -890,11 +847,54 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -948,7 +948,7 @@
         <xdr:cNvPr id="3" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA4F558B-8D56-430D-AA83-772AD1DE26DE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA4F558B-8D56-430D-AA83-772AD1DE26DE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1050,7 +1050,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1083,9 +1083,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1118,6 +1135,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1293,17 +1327,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:T39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.65" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.44140625" customWidth="1"/>
     <col min="2" max="2" width="24.77734375" customWidth="1"/>
@@ -1323,72 +1357,72 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="83"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="14.7" x14ac:dyDescent="0.3">
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+    </row>
+    <row r="4" spans="1:19" ht="14.7" x14ac:dyDescent="0.3">
       <c r="D4" s="2"/>
-      <c r="E4" s="84" t="s">
+      <c r="E4" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
       <c r="J4" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="L4" s="85" t="s">
+      <c r="L4" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="85"/>
-      <c r="N4" s="85"/>
+      <c r="M4" s="70"/>
+      <c r="N4" s="70"/>
       <c r="O4" s="4">
         <v>0.25</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="14.7" x14ac:dyDescent="0.3">
       <c r="D5" s="2"/>
-      <c r="E5" s="84" t="s">
+      <c r="E5" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="85"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
       <c r="J5" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="L5" s="85" t="s">
+      <c r="L5" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="M5" s="85"/>
-      <c r="N5" s="85"/>
+      <c r="M5" s="70"/>
+      <c r="N5" s="70"/>
       <c r="O5" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" ht="14.7" x14ac:dyDescent="0.3">
       <c r="D6" s="2"/>
-      <c r="E6" s="84" t="s">
+      <c r="E6" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="85"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="70"/>
       <c r="J6" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="L6" s="85" t="s">
+      <c r="L6" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="M6" s="85"/>
-      <c r="N6" s="85"/>
+      <c r="M6" s="70"/>
+      <c r="N6" s="70"/>
       <c r="O6" s="5">
         <v>0.7</v>
       </c>
@@ -1397,82 +1431,82 @@
       </c>
       <c r="Q6" s="6"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="E7" s="85" t="s">
+    <row r="7" spans="1:19" ht="14.7" x14ac:dyDescent="0.3">
+      <c r="E7" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="85"/>
-      <c r="G7" s="85"/>
-      <c r="H7" s="85"/>
-      <c r="I7" s="85"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="70"/>
       <c r="J7" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="L7" s="85" t="s">
+      <c r="L7" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="85"/>
-      <c r="N7" s="85"/>
+      <c r="M7" s="70"/>
+      <c r="N7" s="70"/>
       <c r="O7" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" ht="14.7" x14ac:dyDescent="0.3">
       <c r="J8" s="2"/>
       <c r="O8" s="7"/>
     </row>
-    <row r="9" spans="1:19" ht="15.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:19" ht="15.3" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="10" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="86" t="s">
+      <c r="A10" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="87"/>
-      <c r="C10" s="87"/>
-      <c r="D10" s="87"/>
-      <c r="E10" s="87"/>
-      <c r="F10" s="87"/>
-      <c r="G10" s="87"/>
-      <c r="H10" s="87"/>
-      <c r="I10" s="87"/>
-      <c r="J10" s="87"/>
-      <c r="K10" s="87"/>
-      <c r="L10" s="87"/>
-      <c r="M10" s="87"/>
-      <c r="N10" s="87"/>
-      <c r="O10" s="87"/>
-      <c r="P10" s="87"/>
-      <c r="Q10" s="87"/>
-      <c r="R10" s="87"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="72"/>
+      <c r="D10" s="72"/>
+      <c r="E10" s="72"/>
+      <c r="F10" s="72"/>
+      <c r="G10" s="72"/>
+      <c r="H10" s="72"/>
+      <c r="I10" s="72"/>
+      <c r="J10" s="72"/>
+      <c r="K10" s="72"/>
+      <c r="L10" s="72"/>
+      <c r="M10" s="72"/>
+      <c r="N10" s="72"/>
+      <c r="O10" s="72"/>
+      <c r="P10" s="72"/>
+      <c r="Q10" s="72"/>
+      <c r="R10" s="72"/>
       <c r="S10" s="8"/>
     </row>
     <row r="12" spans="1:19" ht="15.9" x14ac:dyDescent="0.3">
-      <c r="D12" s="88" t="s">
+      <c r="D12" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="88"/>
-      <c r="F12" s="88"/>
-      <c r="G12" s="88"/>
-      <c r="H12" s="88"/>
-      <c r="I12" s="88"/>
-      <c r="J12" s="89" t="s">
+      <c r="E12" s="64"/>
+      <c r="F12" s="64"/>
+      <c r="G12" s="64"/>
+      <c r="H12" s="64"/>
+      <c r="I12" s="64"/>
+      <c r="J12" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="89"/>
-      <c r="L12" s="89"/>
-      <c r="M12" s="89"/>
-      <c r="N12" s="89"/>
-      <c r="O12" s="89"/>
-      <c r="P12" s="89"/>
-      <c r="Q12" s="89"/>
-      <c r="R12" s="89"/>
+      <c r="K12" s="65"/>
+      <c r="L12" s="65"/>
+      <c r="M12" s="65"/>
+      <c r="N12" s="65"/>
+      <c r="O12" s="65"/>
+      <c r="P12" s="65"/>
+      <c r="Q12" s="65"/>
+      <c r="R12" s="65"/>
       <c r="S12" s="9"/>
     </row>
     <row r="13" spans="1:19" s="14" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="79" t="s">
+      <c r="A13" s="80" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="79"/>
-      <c r="C13" s="79"/>
+      <c r="B13" s="80"/>
+      <c r="C13" s="80"/>
       <c r="D13" s="46" t="s">
         <v>55</v>
       </c>
@@ -1523,11 +1557,11 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" s="80" t="s">
+      <c r="A14" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="81"/>
-      <c r="C14" s="82"/>
+      <c r="B14" s="67"/>
+      <c r="C14" s="68"/>
       <c r="D14" s="15">
         <v>0</v>
       </c>
@@ -1581,12 +1615,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" s="80" t="s">
+    <row r="15" spans="1:19" ht="14.7" x14ac:dyDescent="0.3">
+      <c r="A15" s="66" t="s">
         <v>82</v>
       </c>
-      <c r="B15" s="81"/>
-      <c r="C15" s="82"/>
+      <c r="B15" s="67"/>
+      <c r="C15" s="68"/>
       <c r="D15" s="15">
         <v>0</v>
       </c>
@@ -1640,12 +1674,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" s="80" t="s">
+    <row r="16" spans="1:19" ht="14.7" x14ac:dyDescent="0.3">
+      <c r="A16" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="81"/>
-      <c r="C16" s="82"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="68"/>
       <c r="D16" s="15">
         <v>0</v>
       </c>
@@ -1699,12 +1733,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A17" s="80" t="s">
+    <row r="17" spans="1:20" ht="14.7" x14ac:dyDescent="0.3">
+      <c r="A17" s="66" t="s">
         <v>83</v>
       </c>
-      <c r="B17" s="81"/>
-      <c r="C17" s="82"/>
+      <c r="B17" s="67"/>
+      <c r="C17" s="68"/>
       <c r="D17" s="15">
         <v>0</v>
       </c>
@@ -1756,12 +1790,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A18" s="80" t="s">
+    <row r="18" spans="1:20" ht="14.7" x14ac:dyDescent="0.3">
+      <c r="A18" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="B18" s="81"/>
-      <c r="C18" s="82"/>
+      <c r="B18" s="67"/>
+      <c r="C18" s="68"/>
       <c r="D18" s="15">
         <v>0</v>
       </c>
@@ -1815,12 +1849,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A19" s="80" t="s">
+    <row r="19" spans="1:20" ht="14.7" x14ac:dyDescent="0.3">
+      <c r="A19" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="B19" s="81"/>
-      <c r="C19" s="82"/>
+      <c r="B19" s="67"/>
+      <c r="C19" s="68"/>
       <c r="D19" s="15">
         <v>0</v>
       </c>
@@ -1874,12 +1908,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A20" s="80" t="s">
+    <row r="20" spans="1:20" ht="14.7" x14ac:dyDescent="0.3">
+      <c r="A20" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="B20" s="81"/>
-      <c r="C20" s="82"/>
+      <c r="B20" s="67"/>
+      <c r="C20" s="68"/>
       <c r="D20" s="15">
         <v>0</v>
       </c>
@@ -1933,12 +1967,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A21" s="80" t="s">
+    <row r="21" spans="1:20" ht="14.7" x14ac:dyDescent="0.3">
+      <c r="A21" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="B21" s="81"/>
-      <c r="C21" s="82"/>
+      <c r="B21" s="67"/>
+      <c r="C21" s="68"/>
       <c r="D21" s="15">
         <v>0</v>
       </c>
@@ -1990,12 +2024,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A22" s="80" t="s">
+    <row r="22" spans="1:20" ht="14.7" x14ac:dyDescent="0.3">
+      <c r="A22" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="81"/>
-      <c r="C22" s="82"/>
+      <c r="B22" s="67"/>
+      <c r="C22" s="68"/>
       <c r="D22" s="15">
         <v>0</v>
       </c>
@@ -2047,12 +2081,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A23" s="76" t="s">
+    <row r="23" spans="1:20" ht="14.7" x14ac:dyDescent="0.3">
+      <c r="A23" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="76"/>
-      <c r="C23" s="76"/>
+      <c r="B23" s="75"/>
+      <c r="C23" s="75"/>
       <c r="D23" s="15">
         <f t="shared" ref="D23:S23" si="6">SUM(D14:D22)</f>
         <v>0</v>
@@ -2119,7 +2153,7 @@
       </c>
       <c r="T23" s="23"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" ht="14.7" x14ac:dyDescent="0.3">
       <c r="A24" s="24"/>
       <c r="B24" s="24"/>
       <c r="C24" s="24"/>
@@ -2130,22 +2164,18 @@
       <c r="H24" s="25"/>
       <c r="I24" s="25"/>
       <c r="J24" s="23"/>
-      <c r="K24" s="62" t="s">
-        <v>94</v>
-      </c>
+      <c r="K24" s="62"/>
       <c r="L24" s="23"/>
       <c r="M24" s="23"/>
       <c r="N24" s="23"/>
       <c r="O24" s="23"/>
       <c r="P24" s="23"/>
       <c r="Q24" s="23"/>
-      <c r="R24" s="62" t="s">
-        <v>95</v>
-      </c>
+      <c r="R24" s="62"/>
       <c r="S24" s="23"/>
       <c r="T24" s="23"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" ht="14.7" x14ac:dyDescent="0.3">
       <c r="A25" s="24"/>
       <c r="B25" s="24"/>
       <c r="C25" s="24"/>
@@ -2172,31 +2202,31 @@
       <c r="S25" s="23"/>
       <c r="T25" s="23"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" ht="14.7" x14ac:dyDescent="0.3">
       <c r="A26" s="30"/>
       <c r="S26" s="31"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A27" s="75" t="s">
+    <row r="27" spans="1:20" ht="14.7" x14ac:dyDescent="0.3">
+      <c r="A27" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="75"/>
-      <c r="C27" s="75"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="75"/>
-      <c r="F27" s="75"/>
-      <c r="G27" s="75"/>
-      <c r="H27" s="75"/>
-      <c r="I27" s="75"/>
-      <c r="J27" s="75"/>
-      <c r="K27" s="75"/>
-      <c r="L27" s="75"/>
-      <c r="M27" s="75"/>
-      <c r="N27" s="75"/>
-      <c r="O27" s="75"/>
-      <c r="P27" s="75"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B27" s="74"/>
+      <c r="C27" s="74"/>
+      <c r="D27" s="74"/>
+      <c r="E27" s="74"/>
+      <c r="F27" s="74"/>
+      <c r="G27" s="74"/>
+      <c r="H27" s="74"/>
+      <c r="I27" s="74"/>
+      <c r="J27" s="74"/>
+      <c r="K27" s="74"/>
+      <c r="L27" s="74"/>
+      <c r="M27" s="74"/>
+      <c r="N27" s="74"/>
+      <c r="O27" s="74"/>
+      <c r="P27" s="74"/>
+    </row>
+    <row r="28" spans="1:20" ht="14.7" x14ac:dyDescent="0.3">
       <c r="A28" s="32"/>
       <c r="B28" s="32"/>
       <c r="C28" s="32"/>
@@ -2214,7 +2244,7 @@
       <c r="O28" s="32"/>
       <c r="P28" s="32"/>
     </row>
-    <row r="29" spans="1:20" ht="41.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="32" t="s">
         <v>31</v>
       </c>
@@ -2234,104 +2264,104 @@
       <c r="O29" s="32"/>
       <c r="P29" s="32"/>
     </row>
-    <row r="30" spans="1:20" ht="41.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="67" t="str">
+    <row r="30" spans="1:20" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="76" t="str">
         <f>CONCATENATE("participant"," ",J6)</f>
         <v>participant VIZLORE</v>
       </c>
-      <c r="B30" s="68"/>
+      <c r="B30" s="77"/>
       <c r="C30" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="77" t="s">
+      <c r="D30" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="E30" s="78"/>
-      <c r="F30" s="78"/>
-      <c r="G30" s="78"/>
-      <c r="H30" s="78"/>
-      <c r="I30" s="78"/>
-      <c r="J30" s="78"/>
-      <c r="K30" s="78"/>
-      <c r="L30" s="78"/>
-      <c r="M30" s="78"/>
-      <c r="N30" s="78"/>
-      <c r="O30" s="78"/>
-      <c r="P30" s="78"/>
+      <c r="E30" s="79"/>
+      <c r="F30" s="79"/>
+      <c r="G30" s="79"/>
+      <c r="H30" s="79"/>
+      <c r="I30" s="79"/>
+      <c r="J30" s="79"/>
+      <c r="K30" s="79"/>
+      <c r="L30" s="79"/>
+      <c r="M30" s="79"/>
+      <c r="N30" s="79"/>
+      <c r="O30" s="79"/>
+      <c r="P30" s="79"/>
     </row>
     <row r="31" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="64" t="s">
+      <c r="A31" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="64"/>
+      <c r="B31" s="81"/>
       <c r="C31" s="61" t="s">
-        <v>91</v>
-      </c>
-      <c r="D31" s="71" t="s">
+        <v>95</v>
+      </c>
+      <c r="D31" s="82" t="s">
         <v>89</v>
       </c>
-      <c r="E31" s="66"/>
-      <c r="F31" s="66"/>
-      <c r="G31" s="66"/>
-      <c r="H31" s="66"/>
-      <c r="I31" s="66"/>
-      <c r="J31" s="66"/>
-      <c r="K31" s="66"/>
-      <c r="L31" s="66"/>
-      <c r="M31" s="66"/>
-      <c r="N31" s="66"/>
-      <c r="O31" s="66"/>
-      <c r="P31" s="66"/>
+      <c r="E31" s="83"/>
+      <c r="F31" s="83"/>
+      <c r="G31" s="83"/>
+      <c r="H31" s="83"/>
+      <c r="I31" s="83"/>
+      <c r="J31" s="83"/>
+      <c r="K31" s="83"/>
+      <c r="L31" s="83"/>
+      <c r="M31" s="83"/>
+      <c r="N31" s="83"/>
+      <c r="O31" s="83"/>
+      <c r="P31" s="83"/>
       <c r="S31" s="31"/>
     </row>
-    <row r="32" spans="1:20" ht="29.3" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="64" t="s">
+    <row r="32" spans="1:20" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="64"/>
+      <c r="B32" s="81"/>
       <c r="C32" s="34">
         <v>62550</v>
       </c>
-      <c r="D32" s="66" t="s">
+      <c r="D32" s="83" t="s">
         <v>90</v>
       </c>
-      <c r="E32" s="66"/>
-      <c r="F32" s="66"/>
-      <c r="G32" s="66"/>
-      <c r="H32" s="66"/>
-      <c r="I32" s="66"/>
-      <c r="J32" s="66"/>
-      <c r="K32" s="66"/>
-      <c r="L32" s="66"/>
-      <c r="M32" s="66"/>
-      <c r="N32" s="66"/>
-      <c r="O32" s="66"/>
-      <c r="P32" s="66"/>
+      <c r="E32" s="83"/>
+      <c r="F32" s="83"/>
+      <c r="G32" s="83"/>
+      <c r="H32" s="83"/>
+      <c r="I32" s="83"/>
+      <c r="J32" s="83"/>
+      <c r="K32" s="83"/>
+      <c r="L32" s="83"/>
+      <c r="M32" s="83"/>
+      <c r="N32" s="83"/>
+      <c r="O32" s="83"/>
+      <c r="P32" s="83"/>
       <c r="S32" s="31"/>
     </row>
-    <row r="33" spans="1:19" ht="31.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="64" t="s">
+    <row r="33" spans="1:19" ht="31.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="64"/>
+      <c r="B33" s="81"/>
       <c r="C33" s="34">
         <v>40000</v>
       </c>
-      <c r="D33" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="E33" s="66"/>
-      <c r="F33" s="66"/>
-      <c r="G33" s="66"/>
-      <c r="H33" s="66"/>
-      <c r="I33" s="66"/>
-      <c r="J33" s="66"/>
-      <c r="K33" s="66"/>
-      <c r="L33" s="66"/>
-      <c r="M33" s="66"/>
-      <c r="N33" s="66"/>
-      <c r="O33" s="66"/>
-      <c r="P33" s="66"/>
+      <c r="D33" s="83" t="s">
+        <v>91</v>
+      </c>
+      <c r="E33" s="83"/>
+      <c r="F33" s="83"/>
+      <c r="G33" s="83"/>
+      <c r="H33" s="83"/>
+      <c r="I33" s="83"/>
+      <c r="J33" s="83"/>
+      <c r="K33" s="83"/>
+      <c r="L33" s="83"/>
+      <c r="M33" s="83"/>
+      <c r="N33" s="83"/>
+      <c r="O33" s="83"/>
+      <c r="P33" s="83"/>
       <c r="S33" s="31"/>
     </row>
     <row r="34" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.3">
@@ -2365,99 +2395,99 @@
       <c r="P35" s="37"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A36" s="67" t="str">
+      <c r="A36" s="76" t="str">
         <f>CONCATENATE("participant"," ",C9)</f>
         <v xml:space="preserve">participant </v>
       </c>
-      <c r="B36" s="68"/>
+      <c r="B36" s="77"/>
       <c r="C36" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D36" s="69" t="s">
+      <c r="D36" s="88" t="s">
         <v>33</v>
       </c>
-      <c r="E36" s="70"/>
-      <c r="F36" s="70"/>
-      <c r="G36" s="70"/>
-      <c r="H36" s="70"/>
-      <c r="I36" s="70"/>
-      <c r="J36" s="70"/>
-      <c r="K36" s="70"/>
-      <c r="L36" s="70"/>
-      <c r="M36" s="70"/>
-      <c r="N36" s="70"/>
-      <c r="O36" s="70"/>
-      <c r="P36" s="70"/>
-    </row>
-    <row r="37" spans="1:19" ht="27.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="64" t="s">
+      <c r="E36" s="89"/>
+      <c r="F36" s="89"/>
+      <c r="G36" s="89"/>
+      <c r="H36" s="89"/>
+      <c r="I36" s="89"/>
+      <c r="J36" s="89"/>
+      <c r="K36" s="89"/>
+      <c r="L36" s="89"/>
+      <c r="M36" s="89"/>
+      <c r="N36" s="89"/>
+      <c r="O36" s="89"/>
+      <c r="P36" s="89"/>
+    </row>
+    <row r="37" spans="1:19" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="64"/>
+      <c r="B37" s="81"/>
       <c r="C37" s="34">
         <v>9000</v>
       </c>
-      <c r="D37" s="65" t="s">
-        <v>93</v>
-      </c>
-      <c r="E37" s="66"/>
-      <c r="F37" s="66"/>
-      <c r="G37" s="66"/>
-      <c r="H37" s="66"/>
-      <c r="I37" s="66"/>
-      <c r="J37" s="66"/>
-      <c r="K37" s="66"/>
-      <c r="L37" s="66"/>
-      <c r="M37" s="66"/>
-      <c r="N37" s="66"/>
-      <c r="O37" s="66"/>
-      <c r="P37" s="66"/>
+      <c r="D37" s="87" t="s">
+        <v>92</v>
+      </c>
+      <c r="E37" s="83"/>
+      <c r="F37" s="83"/>
+      <c r="G37" s="83"/>
+      <c r="H37" s="83"/>
+      <c r="I37" s="83"/>
+      <c r="J37" s="83"/>
+      <c r="K37" s="83"/>
+      <c r="L37" s="83"/>
+      <c r="M37" s="83"/>
+      <c r="N37" s="83"/>
+      <c r="O37" s="83"/>
+      <c r="P37" s="83"/>
       <c r="S37" s="31"/>
     </row>
     <row r="38" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="64" t="s">
+      <c r="A38" s="81" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="64"/>
+      <c r="B38" s="81"/>
       <c r="C38" s="34">
         <v>0</v>
       </c>
-      <c r="D38" s="72"/>
-      <c r="E38" s="73"/>
-      <c r="F38" s="73"/>
-      <c r="G38" s="73"/>
-      <c r="H38" s="73"/>
-      <c r="I38" s="73"/>
-      <c r="J38" s="73"/>
-      <c r="K38" s="73"/>
-      <c r="L38" s="73"/>
-      <c r="M38" s="73"/>
-      <c r="N38" s="73"/>
-      <c r="O38" s="73"/>
-      <c r="P38" s="74"/>
+      <c r="D38" s="84"/>
+      <c r="E38" s="85"/>
+      <c r="F38" s="85"/>
+      <c r="G38" s="85"/>
+      <c r="H38" s="85"/>
+      <c r="I38" s="85"/>
+      <c r="J38" s="85"/>
+      <c r="K38" s="85"/>
+      <c r="L38" s="85"/>
+      <c r="M38" s="85"/>
+      <c r="N38" s="85"/>
+      <c r="O38" s="85"/>
+      <c r="P38" s="86"/>
       <c r="S38" s="31"/>
     </row>
     <row r="39" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="64" t="s">
+      <c r="A39" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="64"/>
+      <c r="B39" s="81"/>
       <c r="C39" s="34">
         <v>0</v>
       </c>
-      <c r="D39" s="65"/>
-      <c r="E39" s="66"/>
-      <c r="F39" s="66"/>
-      <c r="G39" s="66"/>
-      <c r="H39" s="66"/>
-      <c r="I39" s="66"/>
-      <c r="J39" s="66"/>
-      <c r="K39" s="66"/>
-      <c r="L39" s="66"/>
-      <c r="M39" s="66"/>
-      <c r="N39" s="66"/>
-      <c r="O39" s="66"/>
-      <c r="P39" s="66"/>
+      <c r="D39" s="87"/>
+      <c r="E39" s="83"/>
+      <c r="F39" s="83"/>
+      <c r="G39" s="83"/>
+      <c r="H39" s="83"/>
+      <c r="I39" s="83"/>
+      <c r="J39" s="83"/>
+      <c r="K39" s="83"/>
+      <c r="L39" s="83"/>
+      <c r="M39" s="83"/>
+      <c r="N39" s="83"/>
+      <c r="O39" s="83"/>
+      <c r="P39" s="83"/>
       <c r="S39" s="31"/>
     </row>
   </sheetData>
@@ -2467,23 +2497,20 @@
     <protectedRange sqref="D37:P39" name="Range1_2"/>
   </protectedRanges>
   <mergeCells count="40">
-    <mergeCell ref="D12:I12"/>
-    <mergeCell ref="J12:R12"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="E6:I6"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="E7:I7"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="A10:R10"/>
-    <mergeCell ref="E3:I3"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="E5:I5"/>
-    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:P39"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:P33"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:P36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:P37"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:P31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:P32"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:P38"/>
     <mergeCell ref="A27:P27"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A30:B30"/>
@@ -2493,20 +2520,23 @@
     <mergeCell ref="A21:C21"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:P31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:P32"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:P38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:P39"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:P33"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:P36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:P37"/>
+    <mergeCell ref="E3:I3"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="E5:I5"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="E6:I6"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="E7:I7"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="A10:R10"/>
+    <mergeCell ref="D12:I12"/>
+    <mergeCell ref="J12:R12"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A15:C15"/>
   </mergeCells>
   <conditionalFormatting sqref="O4">
     <cfRule type="expression" dxfId="0" priority="1">
@@ -2514,7 +2544,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O6" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"70%, 100%"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2525,14 +2555,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P46"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.65" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.77734375" customWidth="1"/>
     <col min="3" max="3" width="11.5546875" customWidth="1"/>
@@ -2541,8 +2571,8 @@
     <col min="7" max="7" width="17.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:16" ht="18.95" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16" ht="15.3" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:16" ht="18.899999999999999" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="90" t="s">
         <v>40</v>
       </c>
@@ -2552,7 +2582,7 @@
         <v>27240</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="156.19999999999999" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="156.15" x14ac:dyDescent="0.3">
       <c r="B4" s="57" t="s">
         <v>48</v>
       </c>
@@ -2602,7 +2632,7 @@
     <row r="5" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
       <c r="A5" s="60"/>
       <c r="B5" s="63" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C5" s="58" t="s">
         <v>63</v>
@@ -2617,7 +2647,7 @@
         <v>66</v>
       </c>
       <c r="G5" s="63" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H5" s="63">
         <v>1</v>
@@ -2762,7 +2792,7 @@
         <v>3210</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="59"/>
       <c r="B9" s="63" t="s">
         <v>58</v>
@@ -3101,7 +3131,7 @@
       <c r="O23" s="48"/>
       <c r="P23" s="48"/>
     </row>
-    <row r="24" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="55"/>
       <c r="B24" s="55"/>
       <c r="C24" s="58"/>
@@ -3119,7 +3149,7 @@
       <c r="O24" s="48"/>
       <c r="P24" s="48"/>
     </row>
-    <row r="25" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="55"/>
       <c r="B25" s="55"/>
       <c r="C25" s="58"/>
@@ -3137,7 +3167,7 @@
       <c r="O25" s="48"/>
       <c r="P25" s="48"/>
     </row>
-    <row r="26" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="55"/>
       <c r="B26" s="55"/>
       <c r="C26" s="59"/>
@@ -3155,7 +3185,7 @@
       <c r="O26" s="48"/>
       <c r="P26" s="48"/>
     </row>
-    <row r="27" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="55"/>
       <c r="B27" s="55"/>
       <c r="C27" s="58"/>
@@ -3173,7 +3203,7 @@
       <c r="O27" s="48"/>
       <c r="P27" s="38"/>
     </row>
-    <row r="28" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="55"/>
       <c r="B28" s="55"/>
       <c r="C28" s="58"/>
@@ -3191,7 +3221,7 @@
       <c r="O28" s="48"/>
       <c r="P28" s="38"/>
     </row>
-    <row r="29" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="55"/>
       <c r="B29" s="55"/>
       <c r="C29" s="58"/>
@@ -3209,7 +3239,7 @@
       <c r="O29" s="48"/>
       <c r="P29" s="38"/>
     </row>
-    <row r="30" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="55"/>
       <c r="B30" s="55"/>
       <c r="C30" s="59"/>
@@ -3227,7 +3257,7 @@
       <c r="O30" s="48"/>
       <c r="P30" s="38"/>
     </row>
-    <row r="31" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="55"/>
       <c r="B31" s="55"/>
       <c r="C31" s="59"/>
@@ -3245,7 +3275,7 @@
       <c r="O31" s="38"/>
       <c r="P31" s="38"/>
     </row>
-    <row r="32" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="55"/>
       <c r="B32" s="55"/>
       <c r="C32" s="58"/>
@@ -3263,7 +3293,7 @@
       <c r="O32" s="38"/>
       <c r="P32" s="38"/>
     </row>
-    <row r="33" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="55"/>
       <c r="B33" s="55"/>
       <c r="C33" s="58"/>
@@ -3281,7 +3311,7 @@
       <c r="O33" s="38"/>
       <c r="P33" s="38"/>
     </row>
-    <row r="34" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="55"/>
       <c r="B34" s="55"/>
       <c r="C34" s="58"/>
@@ -3299,7 +3329,7 @@
       <c r="O34" s="48"/>
       <c r="P34" s="48"/>
     </row>
-    <row r="35" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="55"/>
       <c r="B35" s="55"/>
       <c r="C35" s="59"/>
@@ -3335,7 +3365,7 @@
       <c r="O36" s="48"/>
       <c r="P36" s="48"/>
     </row>
-    <row r="37" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="55"/>
       <c r="B37" s="55"/>
       <c r="C37" s="59"/>
@@ -3353,7 +3383,7 @@
       <c r="O37" s="48"/>
       <c r="P37" s="48"/>
     </row>
-    <row r="38" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="55"/>
       <c r="B38" s="55"/>
       <c r="C38" s="58"/>
@@ -3371,7 +3401,7 @@
       <c r="O38" s="48"/>
       <c r="P38" s="48"/>
     </row>
-    <row r="39" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="55"/>
       <c r="B39" s="55"/>
       <c r="C39" s="58"/>
@@ -3389,7 +3419,7 @@
       <c r="O39" s="48"/>
       <c r="P39" s="48"/>
     </row>
-    <row r="40" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="55"/>
       <c r="B40" s="55"/>
       <c r="C40" s="59"/>
@@ -3425,7 +3455,7 @@
       <c r="O41" s="48"/>
       <c r="P41" s="48"/>
     </row>
-    <row r="42" spans="1:16" ht="15.9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="55"/>
       <c r="B42" s="55"/>
       <c r="C42" s="58"/>
@@ -3525,14 +3555,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:I35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.65" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18.5546875" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" customWidth="1"/>
@@ -3542,8 +3572,8 @@
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:9" ht="18.95" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:9" ht="15.3" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:9" ht="18.899999999999999" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="90" t="s">
         <v>40</v>
       </c>
@@ -3579,7 +3609,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B5" s="53" t="s">
         <v>57</v>
       </c>
@@ -3605,7 +3635,7 @@
         <v>4250</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B6" s="55" t="s">
         <v>57</v>
       </c>
@@ -3631,7 +3661,7 @@
         <v>3750</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B7" s="53" t="s">
         <v>59</v>
       </c>
@@ -3658,7 +3688,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B8" s="53" t="s">
         <v>58</v>
       </c>
@@ -3685,7 +3715,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B9" s="53" t="s">
         <v>58</v>
       </c>
@@ -3712,7 +3742,7 @@
         <v>3750</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B10" s="55" t="s">
         <v>76</v>
       </c>
@@ -3738,7 +3768,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B11" s="38"/>
       <c r="C11" s="38"/>
       <c r="D11" s="38"/>
@@ -3751,7 +3781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B12" s="38"/>
       <c r="C12" s="38"/>
       <c r="D12" s="38"/>
@@ -3764,7 +3794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B13" s="38"/>
       <c r="C13" s="38"/>
       <c r="D13" s="38"/>
@@ -3777,7 +3807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B14" s="38"/>
       <c r="C14" s="38"/>
       <c r="D14" s="38"/>
@@ -3790,7 +3820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B15" s="38"/>
       <c r="C15" s="38"/>
       <c r="D15" s="38"/>
@@ -3803,7 +3833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B16" s="38"/>
       <c r="C16" s="38"/>
       <c r="D16" s="38"/>
@@ -3816,7 +3846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B17" s="38"/>
       <c r="C17" s="38"/>
       <c r="D17" s="38"/>
@@ -3829,7 +3859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B18" s="38"/>
       <c r="C18" s="38"/>
       <c r="D18" s="38"/>
@@ -3842,7 +3872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B19" s="38"/>
       <c r="C19" s="38"/>
       <c r="D19" s="38"/>
@@ -3855,7 +3885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B20" s="38"/>
       <c r="C20" s="38"/>
       <c r="D20" s="38"/>
@@ -3868,7 +3898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B21" s="38"/>
       <c r="C21" s="38"/>
       <c r="D21" s="38"/>
@@ -3881,7 +3911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B22" s="38"/>
       <c r="C22" s="38"/>
       <c r="D22" s="38"/>
@@ -3894,7 +3924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B23" s="38"/>
       <c r="C23" s="38"/>
       <c r="D23" s="38"/>
@@ -3907,7 +3937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B24" s="38"/>
       <c r="C24" s="38"/>
       <c r="D24" s="38"/>
@@ -3920,7 +3950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B25" s="38"/>
       <c r="C25" s="38"/>
       <c r="D25" s="38"/>
@@ -3933,7 +3963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B26" s="38"/>
       <c r="C26" s="38"/>
       <c r="D26" s="38"/>
@@ -3946,7 +3976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B27" s="38"/>
       <c r="C27" s="38"/>
       <c r="D27" s="38"/>
@@ -4072,14 +4102,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.65" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18.5546875" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
@@ -4088,8 +4118,8 @@
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:9" ht="18.95" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:9" ht="15.3" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:9" ht="18.899999999999999" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="90" t="s">
         <v>40</v>
       </c>
@@ -4152,7 +4182,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B6" s="47" t="s">
         <v>79</v>
       </c>
@@ -4179,7 +4209,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B7" s="53"/>
       <c r="C7" s="53"/>
       <c r="D7" s="53"/>
@@ -4189,7 +4219,7 @@
       <c r="H7" s="53"/>
       <c r="I7" s="53"/>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B8" s="53"/>
       <c r="C8" s="53"/>
       <c r="D8" s="53"/>
@@ -4199,7 +4229,7 @@
       <c r="H8" s="53"/>
       <c r="I8" s="53"/>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B9" s="53"/>
       <c r="C9" s="53"/>
       <c r="D9" s="53"/>
@@ -4209,7 +4239,7 @@
       <c r="H9" s="53"/>
       <c r="I9" s="53"/>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B10" s="53"/>
       <c r="C10" s="49"/>
       <c r="D10" s="49"/>
@@ -4219,7 +4249,7 @@
       <c r="H10" s="49"/>
       <c r="I10" s="38"/>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B11" s="53"/>
       <c r="C11" s="53"/>
       <c r="D11" s="53"/>
@@ -4229,7 +4259,7 @@
       <c r="H11" s="53"/>
       <c r="I11" s="53"/>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B12" s="53"/>
       <c r="C12" s="53"/>
       <c r="D12" s="53"/>
@@ -4239,7 +4269,7 @@
       <c r="H12" s="53"/>
       <c r="I12" s="53"/>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B13" s="38"/>
       <c r="C13" s="49"/>
       <c r="D13" s="49"/>
@@ -4249,7 +4279,7 @@
       <c r="H13" s="49"/>
       <c r="I13" s="38"/>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B14" s="38"/>
       <c r="C14" s="38"/>
       <c r="D14" s="38"/>
@@ -4259,7 +4289,7 @@
       <c r="H14" s="38"/>
       <c r="I14" s="38"/>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B15" s="38"/>
       <c r="C15" s="38"/>
       <c r="D15" s="38"/>
@@ -4269,7 +4299,7 @@
       <c r="H15" s="38"/>
       <c r="I15" s="38"/>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B16" s="38"/>
       <c r="C16" s="38"/>
       <c r="D16" s="38"/>
@@ -4279,7 +4309,7 @@
       <c r="H16" s="38"/>
       <c r="I16" s="38"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B17" s="38"/>
       <c r="C17" s="38"/>
       <c r="D17" s="38"/>
@@ -4289,7 +4319,7 @@
       <c r="H17" s="38"/>
       <c r="I17" s="38"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B18" s="38"/>
       <c r="C18" s="38"/>
       <c r="D18" s="38"/>
@@ -4299,7 +4329,7 @@
       <c r="H18" s="38"/>
       <c r="I18" s="38"/>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B19" s="53"/>
       <c r="C19" s="53"/>
       <c r="D19" s="53"/>
@@ -4309,7 +4339,7 @@
       <c r="H19" s="53"/>
       <c r="I19" s="53"/>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B20" s="53"/>
       <c r="C20" s="53"/>
       <c r="D20" s="53"/>
@@ -4319,7 +4349,7 @@
       <c r="H20" s="53"/>
       <c r="I20" s="53"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B21" s="38"/>
       <c r="C21" s="38"/>
       <c r="D21" s="38"/>
@@ -4329,7 +4359,7 @@
       <c r="H21" s="38"/>
       <c r="I21" s="38"/>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B22" s="38"/>
       <c r="C22" s="38"/>
       <c r="D22" s="38"/>
@@ -4339,7 +4369,7 @@
       <c r="H22" s="38"/>
       <c r="I22" s="38"/>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B23" s="38"/>
       <c r="C23" s="38"/>
       <c r="D23" s="38"/>
@@ -4349,7 +4379,7 @@
       <c r="H23" s="38"/>
       <c r="I23" s="38"/>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B24" s="38"/>
       <c r="C24" s="38"/>
       <c r="D24" s="38"/>
@@ -4359,7 +4389,7 @@
       <c r="H24" s="38"/>
       <c r="I24" s="38"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B25" s="38"/>
       <c r="C25" s="38"/>
       <c r="D25" s="38"/>
@@ -4369,7 +4399,7 @@
       <c r="H25" s="38"/>
       <c r="I25" s="38"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B26" s="38"/>
       <c r="C26" s="38"/>
       <c r="D26" s="38"/>
@@ -4379,7 +4409,7 @@
       <c r="H26" s="38"/>
       <c r="I26" s="38"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:9" ht="14.7" x14ac:dyDescent="0.3">
       <c r="B27" s="38"/>
       <c r="C27" s="38"/>
       <c r="D27" s="38"/>

</xml_diff>